<commit_message>
Add some useful middlewares for rate limiting in requests, compression and security headers
</commit_message>
<xml_diff>
--- a/scouts.xlsx
+++ b/scouts.xlsx
@@ -535,7 +535,7 @@
         <v>eribattaglia@gmail.com</v>
       </c>
       <c r="M2" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O2" t="str">
         <v>Secundario</v>
@@ -609,7 +609,7 @@
         <v>gacaore2@gmail.com</v>
       </c>
       <c r="M3" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O3" t="str">
         <v>Secundario</v>
@@ -683,7 +683,7 @@
         <v>lulaazul2011@gmail.com</v>
       </c>
       <c r="M4" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O4" t="str">
         <v>Secundario</v>
@@ -757,7 +757,7 @@
         <v>agustinguti123@gmail.com</v>
       </c>
       <c r="M5" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O5" t="str">
         <v>Secundario</v>
@@ -831,7 +831,7 @@
         <v>gonzalo.corcuera7@gmail.com</v>
       </c>
       <c r="M6" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O6" t="str">
         <v>Secundario</v>
@@ -902,7 +902,7 @@
         <v>1163004817</v>
       </c>
       <c r="M7" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T7" t="str">
         <v>Argentina</v>
@@ -976,7 +976,7 @@
         <v>1151772755</v>
       </c>
       <c r="M8" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T8" t="str">
         <v>Argentina</v>
@@ -1047,7 +1047,7 @@
         <v>1160198817</v>
       </c>
       <c r="M9" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T9" t="str">
         <v>Argentina</v>
@@ -1118,7 +1118,7 @@
         <v>1170333660</v>
       </c>
       <c r="M10" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O10" t="str">
         <v>Primario</v>
@@ -1192,7 +1192,7 @@
         <v>1126877839</v>
       </c>
       <c r="M11" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T11" t="str">
         <v>Argentina</v>
@@ -1263,7 +1263,7 @@
         <v>1164664874</v>
       </c>
       <c r="M12" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T12" t="str">
         <v>Argentina</v>
@@ -1334,7 +1334,7 @@
         <v>1127204979</v>
       </c>
       <c r="M13" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T13" t="str">
         <v>Argentina</v>
@@ -1405,7 +1405,7 @@
         <v>1165610973</v>
       </c>
       <c r="M14" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T14" t="str">
         <v>Argentina</v>
@@ -1476,7 +1476,7 @@
         <v>1173669087</v>
       </c>
       <c r="M15" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T15" t="str">
         <v>Argentina</v>
@@ -1547,7 +1547,7 @@
         <v>1121935195</v>
       </c>
       <c r="M16" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T16" t="str">
         <v>Argentina</v>
@@ -1618,7 +1618,7 @@
         <v>1134857678</v>
       </c>
       <c r="M17" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T17" t="str">
         <v>Argentina</v>
@@ -1689,7 +1689,7 @@
         <v>1130613307</v>
       </c>
       <c r="M18" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T18" t="str">
         <v>Argentina</v>
@@ -1760,7 +1760,7 @@
         <v>1157096382</v>
       </c>
       <c r="M19" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T19" t="str">
         <v>Argentina</v>
@@ -1828,7 +1828,7 @@
         <v>Soltero</v>
       </c>
       <c r="M20" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O20" t="str">
         <v>Secundario</v>
@@ -1899,7 +1899,7 @@
         <v>Soltero</v>
       </c>
       <c r="M21" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T21" t="str">
         <v>Argentina</v>
@@ -1970,7 +1970,7 @@
         <v>1130617220</v>
       </c>
       <c r="M22" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T22" t="str">
         <v>Argentina</v>
@@ -2041,7 +2041,7 @@
         <v>1151763374</v>
       </c>
       <c r="M23" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O23" t="str">
         <v>Primario</v>
@@ -2115,7 +2115,7 @@
         <v>1171295213</v>
       </c>
       <c r="M24" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T24" t="str">
         <v>Argentina</v>
@@ -2186,7 +2186,7 @@
         <v>1127308348</v>
       </c>
       <c r="M25" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T25" t="str">
         <v>Argentina</v>
@@ -2257,7 +2257,7 @@
         <v>1132158264</v>
       </c>
       <c r="M26" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O26" t="str">
         <v>Primario</v>
@@ -2331,7 +2331,7 @@
         <v>1153781104</v>
       </c>
       <c r="M27" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T27" t="str">
         <v>Argentina</v>
@@ -2402,7 +2402,7 @@
         <v>1125150663</v>
       </c>
       <c r="M28" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O28" t="str">
         <v>Primario</v>
@@ -2479,7 +2479,7 @@
         <v>1168323602</v>
       </c>
       <c r="M29" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O29" t="str">
         <v>Primario</v>
@@ -2550,7 +2550,7 @@
         <v>Soltero</v>
       </c>
       <c r="M30" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="T30" t="str">
         <v>Argentina</v>
@@ -2618,7 +2618,7 @@
         <v>1125724676</v>
       </c>
       <c r="M31" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O31" t="str">
         <v>Primario</v>
@@ -2689,7 +2689,7 @@
         <v>1122544269</v>
       </c>
       <c r="M32" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O32" t="str">
         <v>Primario</v>
@@ -2754,7 +2754,7 @@
         <v>Soltero</v>
       </c>
       <c r="M33" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O33" t="str">
         <v>Primario</v>
@@ -2822,7 +2822,7 @@
         <v>Soltero</v>
       </c>
       <c r="M34" t="str">
-        <v>Catolicismo</v>
+        <v>Catolica</v>
       </c>
       <c r="O34" t="str">
         <v>Primario</v>

</xml_diff>